<commit_message>
updates on Checkout tests
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Imad-\git\DSS_Automation\src\com\generic\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D7B276-7880-4271-96C5-D18900B0EC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AD64AA-0940-4B38-8D59-06B0B009528A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1275" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1275" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CheckOutRegression" sheetId="8" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="115">
   <si>
     <t>runTest</t>
   </si>
@@ -148,15 +148,6 @@
     <t>mail</t>
   </si>
   <si>
-    <t>Accept</t>
-  </si>
-  <si>
-    <t>Tester</t>
-  </si>
-  <si>
-    <t>LastVisa</t>
-  </si>
-  <si>
     <t>addressCode</t>
   </si>
   <si>
@@ -196,24 +187,9 @@
     <t>U-09</t>
   </si>
   <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>Ardenham Court</t>
-  </si>
-  <si>
-    <t>HP19 3EQ</t>
-  </si>
-  <si>
-    <t>LONDON</t>
-  </si>
-  <si>
     <t>4725836952</t>
   </si>
   <si>
-    <t>Firstvisa</t>
-  </si>
-  <si>
     <t>U-10</t>
   </si>
   <si>
@@ -230,15 +206,6 @@
   </si>
   <si>
     <t>Ohio</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>14 Tottenham Court Road</t>
-  </si>
-  <si>
-    <t>W1T 1JY</t>
   </si>
   <si>
     <t>card</t>
@@ -413,7 +380,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,11 +438,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Docs-Arimo"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arimo"/>
     </font>
     <font>
       <sz val="11"/>
@@ -668,9 +630,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -752,33 +713,31 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -787,7 +746,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -796,6 +755,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1016,8 +976,8 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1034,199 +994,199 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="28.5">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" s="9" t="s">
+      <c r="F2" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>15</v>
+      <c r="H2" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="28.5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="G3" s="9" t="s">
+      <c r="F3" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>15</v>
+      <c r="H3" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="28.5">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>1</v>
       </c>
-      <c r="F4" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="G4" s="9" t="s">
+      <c r="F4" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>15</v>
+      <c r="H4" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="28.5">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F5" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="G5" s="9" t="s">
+      <c r="C5" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="22" t="s">
-        <v>15</v>
+      <c r="H5" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="28.5">
-      <c r="A6" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="C6" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="G6" s="9" t="s">
+      <c r="F6" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="I6" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>15</v>
+      <c r="H6" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="15" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -1239,51 +1199,51 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="42.75">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="42.75">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1300,7 +1260,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1315,189 +1275,189 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="30" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="48" t="s">
+      <c r="B2" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="48">
+      <c r="F2" s="45">
         <v>12341234</v>
       </c>
-      <c r="G2" s="34" t="s">
-        <v>90</v>
+      <c r="G2" s="48" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="G3" s="34" t="s">
-        <v>92</v>
+      <c r="B3" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>93</v>
+      <c r="B4" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="26"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="G5" s="34" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="36" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="19"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="27"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="36" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="19"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="27"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="20"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="36" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="19"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="20"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="36" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="19"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="20"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="20"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="20"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="19"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="15" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1506,10 +1466,10 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1524,133 +1484,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="G1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="H1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" s="39" t="s">
-        <v>104</v>
+      <c r="B2" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="26" t="s">
+      <c r="E3" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="F3" s="29" t="s">
         <v>57</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>58</v>
       </c>
       <c r="G3" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>59</v>
+      <c r="H3" s="29" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1681,143 +1589,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="12" t="s">
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="B5" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="12" t="s">
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="B6" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" s="42">
+      <c r="B7" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="39">
         <v>1</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="39" t="s">
-        <v>114</v>
+      <c r="F7" s="36" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OMS cases: approve and reject ohr
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Imad-\git\DSS_Automation\src\com\generic\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AD64AA-0940-4B38-8D59-06B0B009528A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA33544-F096-4EFD-80D3-68C1EF34C257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1275" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CheckOutRegression" sheetId="8" r:id="rId1"/>
     <sheet name="PDPRegression" sheetId="11" r:id="rId2"/>
-    <sheet name="users" sheetId="17" r:id="rId3"/>
-    <sheet name="addresses" sheetId="18" r:id="rId4"/>
-    <sheet name="cards" sheetId="19" r:id="rId5"/>
+    <sheet name="OMSAccountRegression" sheetId="20" r:id="rId3"/>
+    <sheet name="users" sheetId="17" r:id="rId4"/>
+    <sheet name="addresses" sheetId="18" r:id="rId5"/>
+    <sheet name="cards" sheetId="19" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="148">
   <si>
     <t>runTest</t>
   </si>
@@ -374,6 +375,105 @@
   </si>
   <si>
     <t>Registered user with multiple addresses</t>
+  </si>
+  <si>
+    <t>Create a Placer account</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Login to the created placer account</t>
+  </si>
+  <si>
+    <t>COB-06</t>
+  </si>
+  <si>
+    <t>Create a Reviewer account</t>
+  </si>
+  <si>
+    <t>Login to the created Reviewer account</t>
+  </si>
+  <si>
+    <t>Login to the created Approver account</t>
+  </si>
+  <si>
+    <t>Login to the created Admin account</t>
+  </si>
+  <si>
+    <t>Create an Approver account</t>
+  </si>
+  <si>
+    <t>Create an Admin account</t>
+  </si>
+  <si>
+    <t>COB-07</t>
+  </si>
+  <si>
+    <t>COB-08</t>
+  </si>
+  <si>
+    <t>admin@mailinator.com</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>dhanireviewer@gmail.com</t>
+  </si>
+  <si>
+    <t>Admin User: Manage Users Order History Validation</t>
+  </si>
+  <si>
+    <t>Admin User: Order History Validation From Manage Users</t>
+  </si>
+  <si>
+    <t>Admin user: Normal Order Validation</t>
+  </si>
+  <si>
+    <t>Reviewer user: Normal Order Validation</t>
+  </si>
+  <si>
+    <t>On Hold Order Review - Submit for approval</t>
+  </si>
+  <si>
+    <t>On Hold Order Approve - Submit for release</t>
+  </si>
+  <si>
+    <t>On Hold Order Review - Reject Order</t>
+  </si>
+  <si>
+    <t>On Hold Order Approve - Reject Order</t>
+  </si>
+  <si>
+    <t>Validate the order is rejected on order history for the placer account after the reviewer rejected</t>
+  </si>
+  <si>
+    <t>Validate the order is rejected on order history for the placer account after the approver rejected</t>
+  </si>
+  <si>
+    <t>COB-09</t>
+  </si>
+  <si>
+    <t>COB-10</t>
+  </si>
+  <si>
+    <t>COB-11</t>
+  </si>
+  <si>
+    <t>COB-12</t>
+  </si>
+  <si>
+    <t>COB-13</t>
+  </si>
+  <si>
+    <t>COB-14</t>
+  </si>
+  <si>
+    <t>COB-15</t>
   </si>
 </sst>
 </file>
@@ -424,12 +524,6 @@
       <name val="Arimo"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arimo"/>
@@ -462,6 +556,10 @@
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -630,7 +728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -680,9 +778,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -690,9 +785,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -705,11 +797,10 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -717,36 +808,24 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -755,7 +834,29 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -977,7 +1078,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1041,16 +1142,16 @@
       <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="36" t="s">
         <v>105</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="I2" s="37" t="s">
         <v>45</v>
       </c>
       <c r="J2" s="9" t="s">
@@ -1073,16 +1174,16 @@
       <c r="E3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="36" t="s">
         <v>106</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="37" t="s">
         <v>45</v>
       </c>
       <c r="J3" s="9" t="s">
@@ -1105,16 +1206,16 @@
       <c r="E4" s="5">
         <v>1</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="36" t="s">
         <v>106</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="42" t="s">
+      <c r="H4" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="42" t="s">
+      <c r="I4" s="37" t="s">
         <v>45</v>
       </c>
       <c r="J4" s="9" t="s">
@@ -1137,19 +1238,19 @@
       <c r="E5" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="36" t="s">
         <v>107</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="19" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1169,24 +1270,24 @@
       <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="F6" s="36" t="s">
         <v>108</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="42" t="s">
+      <c r="H6" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="42" t="s">
+      <c r="I6" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="19" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -1199,7 +1300,7 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1253,6 +1354,443 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBFB6F6C-978D-42F6-9341-FFAE1E74DB9A}">
+  <sheetPr>
+    <tabColor rgb="FF205867"/>
+  </sheetPr>
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="2" width="7.875" customWidth="1"/>
+    <col min="3" max="3" width="30.75" customWidth="1"/>
+    <col min="4" max="4" width="31.875" customWidth="1"/>
+    <col min="5" max="5" width="13.625" customWidth="1"/>
+    <col min="6" max="6" width="17.375" customWidth="1"/>
+    <col min="7" max="7" width="11.875" customWidth="1"/>
+    <col min="8" max="8" width="17.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.5">
+      <c r="A3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.5">
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" s="38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.5">
+      <c r="A10" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.5">
+      <c r="A11" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.5">
+      <c r="A12" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28.5">
+      <c r="A13" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.5">
+      <c r="A14" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="42.75">
+      <c r="A15" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="42.75">
+      <c r="A16" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF002060"/>
@@ -1260,7 +1798,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1275,193 +1813,209 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="27" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="45">
-        <v>12341234</v>
-      </c>
-      <c r="G2" s="48" t="s">
+      <c r="F2" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="28" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="45" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="28" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="45" t="s">
+      <c r="C4" s="47"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="28" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="28" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="26"/>
+      <c r="B6" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="40"/>
+      <c r="F6" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="26"/>
+      <c r="B7" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="47"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="19"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="42"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="19"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="42"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="19"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="42"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="19"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="41"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="19"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="18"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF002060"/>
@@ -1505,59 +2059,59 @@
       <c r="G1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="21" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="31" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="26" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1567,7 +2121,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF002060"/>
@@ -1589,7 +2143,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="32" t="s">
         <v>59</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -1609,122 +2163,122 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="31" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="18" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="34">
         <v>1</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="31" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Checkout tests for iPad and Mobile views. Parallel tests. Report updates.
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Imad-\git\DSS_Automation\src\com\generic\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA33544-F096-4EFD-80D3-68C1EF34C257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EA3700-59AF-4880-A1B0-4A0881B5150C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1020" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CheckOutRegression" sheetId="8" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="157">
   <si>
     <t>runTest</t>
   </si>
@@ -89,21 +89,12 @@
     <t>COB-02</t>
   </si>
   <si>
-    <t>fresh-single</t>
-  </si>
-  <si>
     <t>COB-03</t>
   </si>
   <si>
-    <t>registered-multiple</t>
-  </si>
-  <si>
     <t>COB-04</t>
   </si>
   <si>
-    <t>registered-single</t>
-  </si>
-  <si>
     <t>U-03</t>
   </si>
   <si>
@@ -260,15 +251,6 @@
     <t>Guest user with single item using CC</t>
   </si>
   <si>
-    <t>Guest user with multible items using CC</t>
-  </si>
-  <si>
-    <t>fresh-multible</t>
-  </si>
-  <si>
-    <t>registered-multible</t>
-  </si>
-  <si>
     <t>placer1@gmail.com</t>
   </si>
   <si>
@@ -368,15 +350,9 @@
     <t>COB-05</t>
   </si>
   <si>
-    <t>Registered user  with multible items</t>
-  </si>
-  <si>
     <t>Registered user with single item</t>
   </si>
   <si>
-    <t>Registered user with multiple addresses</t>
-  </si>
-  <si>
     <t>Create a Placer account</t>
   </si>
   <si>
@@ -474,13 +450,64 @@
   </si>
   <si>
     <t>COB-15</t>
+  </si>
+  <si>
+    <t>Guest Cart</t>
+  </si>
+  <si>
+    <t>Registered Cart</t>
+  </si>
+  <si>
+    <t>Registered user with multiple items</t>
+  </si>
+  <si>
+    <t>Registered user  with multiple items</t>
+  </si>
+  <si>
+    <t>Guest user with multiple items using CC</t>
+  </si>
+  <si>
+    <t>registered user -multiple items</t>
+  </si>
+  <si>
+    <t>registered user-single item</t>
+  </si>
+  <si>
+    <t>fresh user - multiple items</t>
+  </si>
+  <si>
+    <t>registered user - multiple items</t>
+  </si>
+  <si>
+    <t>fresh user - single item</t>
+  </si>
+  <si>
+    <t>auto_placer@mailinator.com</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>placer2@gmail.com</t>
+  </si>
+  <si>
+    <t>placer2</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>placer</t>
+  </si>
+  <si>
+    <t>U-01,U-07,U-08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -560,6 +587,12 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -728,7 +761,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -855,6 +888,11 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1075,10 +1113,10 @@
   <sheetPr>
     <tabColor rgb="FF205867"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1126,68 +1164,68 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="28.5">
+    <row r="2" spans="1:10">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>75</v>
+      <c r="C2" s="10" t="s">
+        <v>140</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="37" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I2" s="37" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="28.5">
       <c r="A3" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>21</v>
+      <c r="C3" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>149</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="37" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I3" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>32</v>
+        <v>42</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="28.5">
@@ -1197,93 +1235,157 @@
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="5">
-        <v>1</v>
+      <c r="C4" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="37" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>32</v>
+        <v>42</v>
+      </c>
+      <c r="J4" s="52" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="28.5">
       <c r="A5" s="5" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>74</v>
+        <v>146</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
       </c>
       <c r="F5" s="36" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="37" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I5" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="J5" s="52" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="28.5">
       <c r="A6" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>78</v>
+        <v>147</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="F6" s="36" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I6" s="37" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>32</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="28.5">
+      <c r="A7" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="52" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="52" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1322,30 +1424,30 @@
     </row>
     <row r="2" spans="1:4" ht="42.75">
       <c r="A2" s="13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="42.75">
       <c r="A3" s="13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1360,8 +1462,8 @@
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1405,26 +1507,24 @@
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="B2" s="5"/>
       <c r="C2" s="10" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H2" s="38" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.5">
@@ -1433,19 +1533,19 @@
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="10" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H3" s="19" t="s">
         <v>1</v>
@@ -1453,49 +1553,47 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>1</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B4" s="5"/>
       <c r="C4" s="10" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H4" s="38" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.5">
       <c r="A5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="10" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F5" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H5" s="19" t="s">
         <v>1</v>
@@ -1503,46 +1601,44 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>1</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B6" s="5"/>
       <c r="C6" s="10" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F6" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H6" s="38" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="5" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="10" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>13</v>
@@ -1553,127 +1649,121 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H8" s="38" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="5" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="10" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.5">
       <c r="A10" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>1</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="B10" s="5"/>
       <c r="C10" s="10" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.5">
       <c r="A11" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>1</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="B11" s="5"/>
       <c r="C11" s="10" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.5">
       <c r="A12" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>1</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="B12" s="5"/>
       <c r="C12" s="10" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E12" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H12" s="19" t="s">
         <v>15</v>
@@ -1681,25 +1771,23 @@
     </row>
     <row r="13" spans="1:8" ht="28.5">
       <c r="A13" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>1</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="B13" s="5"/>
       <c r="C13" s="10" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H13" s="19" t="s">
         <v>15</v>
@@ -1707,51 +1795,47 @@
     </row>
     <row r="14" spans="1:8" ht="28.5">
       <c r="A14" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>1</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="B14" s="5"/>
       <c r="C14" s="10" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="42.75">
       <c r="A15" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>1</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="B15" s="5"/>
       <c r="C15" s="10" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H15" s="19" t="s">
         <v>15</v>
@@ -1759,28 +1843,26 @@
     </row>
     <row r="16" spans="1:8" ht="42.75">
       <c r="A16" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>1</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="B16" s="5"/>
       <c r="C16" s="10" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="E16" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1798,7 +1880,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1814,48 +1896,48 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="A1" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="E1" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="F1" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="27" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
       <c r="A2" s="38" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C2" s="48" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E2" s="38" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="38" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
@@ -1863,121 +1945,145 @@
         <v>15</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
       <c r="E3" s="39"/>
       <c r="F3" s="38" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
       <c r="A4" s="38" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C4" s="47"/>
       <c r="D4" s="40"/>
       <c r="E4" s="40"/>
       <c r="F4" s="38" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="38" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="38" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E6" s="40"/>
       <c r="F6" s="38" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="38" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="40"/>
       <c r="E7" s="40"/>
       <c r="F7" s="38" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="42"/>
+        <v>46</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="G8" s="50" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="42"/>
+        <v>47</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="50" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="38" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B10" s="47"/>
       <c r="C10" s="47"/>
@@ -1988,7 +2094,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="43" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B11" s="44"/>
       <c r="C11" s="44"/>
@@ -1999,7 +2105,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
@@ -2039,54 +2145,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="G1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="H1" s="21" t="s">
         <v>41</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B2" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="31" t="s">
         <v>87</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2094,25 +2200,25 @@
         <v>14</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D3" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>58</v>
-      </c>
       <c r="H3" s="26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2144,22 +2250,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2167,99 +2273,99 @@
         <v>13</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F2" s="31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>66</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="30" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D4" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>67</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="30" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2267,7 +2373,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C7" s="34">
         <v>1</v>
@@ -2279,7 +2385,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="31" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>